<commit_message>
Added the main image pipeline for analysis. It runs completely and without errors. The main part of the analysis is COMPLETE!
</commit_message>
<xml_diff>
--- a/Observation_Shifts.xlsx
+++ b/Observation_Shifts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\GitHub\ASTR310Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647CC3A-D3A4-41F5-A770-4F1420AC31A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C753306A-EC98-4FC7-8D79-CC1B01DDA9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{AEFF7B63-F02C-4361-90DE-9F67E8E78FA5}"/>
+    <workbookView xWindow="5760" yWindow="3366" windowWidth="17280" windowHeight="8994" xr2:uid="{AEFF7B63-F02C-4361-90DE-9F67E8E78FA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>